<commit_message>
New lifetable data from National offices of statistics
New lifetable data from National offices of statistics
</commit_message>
<xml_diff>
--- a/Outcomes/Information available for 23 selected countries.xlsx
+++ b/Outcomes/Information available for 23 selected countries.xlsx
@@ -277,6 +277,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -284,7 +285,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,7 +532,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,14 +560,14 @@
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
       <c r="P1" t="s">
         <v>40</v>
       </c>
@@ -652,7 +652,7 @@
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
-      <c r="P3" s="18" t="s">
+      <c r="P3" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -730,7 +730,7 @@
       <c r="N5" s="13">
         <v>1997.99</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -769,7 +769,7 @@
       <c r="N6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -806,7 +806,7 @@
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
-      <c r="P7" s="18" t="s">
+      <c r="P7" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -843,7 +843,7 @@
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -880,7 +880,7 @@
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
-      <c r="P9" s="18" t="s">
+      <c r="P9" s="15" t="s">
         <v>45</v>
       </c>
     </row>
@@ -919,7 +919,7 @@
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
-      <c r="P10" s="18" t="s">
+      <c r="P10" s="15" t="s">
         <v>46</v>
       </c>
     </row>
@@ -956,7 +956,7 @@
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
-      <c r="P11" s="18" t="s">
+      <c r="P11" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -995,7 +995,7 @@
       <c r="N12" s="13">
         <v>1990</v>
       </c>
-      <c r="P12" s="18">
+      <c r="P12" s="15">
         <v>1989</v>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
-      <c r="P13" s="18" t="s">
+      <c r="P13" s="15" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
-      <c r="P14" s="18" t="s">
+      <c r="P14" s="15" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
-      <c r="P15" s="18" t="s">
+      <c r="P15" s="15" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1145,7 +1145,7 @@
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
-      <c r="P16" s="18" t="s">
+      <c r="P16" s="15" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1182,7 +1182,7 @@
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
-      <c r="P17" s="18" t="s">
+      <c r="P17" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1219,7 +1219,7 @@
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
-      <c r="P18" s="18" t="s">
+      <c r="P18" s="15" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
-      <c r="P19" s="18" t="s">
+      <c r="P19" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
-      <c r="P20" s="18" t="s">
+      <c r="P20" s="15" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
-      <c r="P21" s="18" t="s">
+      <c r="P21" s="15" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1369,7 +1369,7 @@
       <c r="N22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="P22" s="18" t="s">
+      <c r="P22" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
-      <c r="P23" s="18" t="s">
+      <c r="P23" s="15" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       <c r="N24" s="13">
         <v>1990</v>
       </c>
-      <c r="P24" s="18" t="s">
+      <c r="P24" s="15" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1488,12 +1488,12 @@
       </c>
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
-      <c r="P25" s="18" t="s">
+      <c r="P25" s="15" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P26" s="18"/>
+      <c r="P26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>